<commit_message>
Ajuste para pegar o site de forma mais correta
</commit_message>
<xml_diff>
--- a/company_data.xlsx
+++ b/company_data.xlsx
@@ -463,14 +463,10 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Rimar Contábil</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>R. Augusto de Vasconcelos, 544 - sala 374 - Campo Grande, Rio de Janeiro - RJ, 23050-340</t>
-        </is>
-      </c>
+          <t>MG Contécnica - Unidade Barra da Tijuca</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -478,60 +474,88 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Samaritana | Escritório de Contabilidade | Assessoria Contábil | Imposto de Renda | Campo Grande</t>
+          <t>AXM</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R. Uruna, 106 - Campo Grande, Rio de Janeiro - RJ, 23045-130</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+          <t>Tv. do Ouvidor, 5 - 4 andar - Centro, Rio de Janeiro - RJ, 20040-040</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>(21) 2206-1000</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>axms.com.br</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Escritório de Gestão e Contabilidade - Lira Araújo Assessoria Contábil Campo Grande</t>
+          <t>Seletus Contabilidade - RJ</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R. Augusto de Vasconcelos, 544 - Sala 445 - Campo Grande, Rio de Janeiro - RJ, 23050-340</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+          <t>R. Campo Grande, 1014 - sala 526 - Campo Grande, Rio de Janeiro - RJ, 23080-000</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>(21) 4107-1417</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>seletuscontabilidade.com.br</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Liberty Assessoria Contábil</t>
+          <t>Seletus Contabilidade - RJ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R. Augusto de Vasconcelos, 544 - Sala 325 - Campo Grande, Rio de Janeiro - RJ, 23050-340</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+          <t>R. Campo Grande, 1014 - sala 526 - Campo Grande, Rio de Janeiro - RJ, 23080-000</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>(21) 4107-1417</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>seletuscontabilidade.com.br</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>G&amp;R Contabilidade Digital</t>
+          <t>Cemage Contabilidade</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R. Augusto de Vasconcelos, 544 - sala 218 - Campo Grande, Rio de Janeiro - RJ, 23050-340</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
+          <t>R. Viúva Dantas, 60 - Campo Grande, Rio de Janeiro - RJ, 23050-090</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>(21) 2413-5334</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Ajuste  na regra do robo
</commit_message>
<xml_diff>
--- a/company_data.xlsx
+++ b/company_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,79 +463,83 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MG Contécnica - Unidade Barra da Tijuca</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+          <t>Be Odonto</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Office Mall Campo Grande - Estrada do Cachamorra, 350. Bloco 1, sala 423 - Campo Grande, Rio de Janeiro - RJ, 23040-150</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>(21) 96681-8555</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>beodontologia.com.br</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AXM</t>
+          <t>Gal Odontologia</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Tv. do Ouvidor, 5 - 4 andar - Centro, Rio de Janeiro - RJ, 20040-040</t>
+          <t>Av. Belmiro Valverde, 87 - Campo Grande, Rio de Janeiro - RJ, 23010-540</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(21) 2206-1000</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>axms.com.br</t>
-        </is>
-      </c>
+          <t>(21) 97469-6436</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Seletus Contabilidade - RJ</t>
+          <t>K.A. Clínica de Odontologia e Estética</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R. Campo Grande, 1014 - sala 526 - Campo Grande, Rio de Janeiro - RJ, 23080-000</t>
+          <t>Estr. do Monteiro, 244 - Sala 207 - Campo Grande, Rio de Janeiro - RJ, 23045-830</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(21) 4107-1417</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>seletuscontabilidade.com.br</t>
-        </is>
-      </c>
+          <t>(21) 97544-0520</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Seletus Contabilidade - RJ</t>
+          <t>Clínica Dra Priscila Máximo - Odontopediatria Campo Grande RJ / Invisalign</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R. Campo Grande, 1014 - sala 526 - Campo Grande, Rio de Janeiro - RJ, 23080-000</t>
+          <t>Av. Maria Teresa, 260 - Bl3 Sl 320 - Campo Grande, Rio de Janeiro - RJ, 23050-160</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>(21) 4107-1417</t>
+          <t>(21) 99883-0999</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>seletuscontabilidade.com.br</t>
+          <t>instagram.com</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -543,21 +547,128 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cemage Contabilidade</t>
+          <t>Odonto Nobre Rio</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R. Viúva Dantas, 60 - Campo Grande, Rio de Janeiro - RJ, 23050-090</t>
+          <t>Estrada da Cachamorra. 350 bl:03 loja:127 - Campo Grande, Rio de Janeiro - RJ, 23040-150</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>(21) 2413-5334</t>
+          <t>(21) 2412-5522</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Dra Graciele Castro - Odontologia</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Estr. da Cachamorra, 350 - bloco 3 sala 204 - Campo Grande, Rio de Janeiro - RJ, 23040-150</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sorrisos Odontologia</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>R. Prof. Castilho, 431 - Loja N - Campo Grande, Rio de Janeiro - RJ, 23045-060</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>(21) 3281-4872</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>sorrisosodontologia.com.br</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Sorrisart - Clínica e Emergência Odontológica</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>R. Augusto de Vasconcelos, 177 - Salas 408 a 410 - Campo Grande, Rio de Janeiro - RJ, 23050-340</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>(21) 97906-4001</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>sorrisart.com</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Odontoclínica Campo Grande</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Rua Coronel Agostinho, 76 2º andar, sobrelojas 206, 213, 215 e 217 - Campo Grande, Rio de Janeiro - RJ, 23050-360</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>(21) 3402-1227</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>odontoclinicacg.com.br</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Multiodonto Clinica Odontológica</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>R. Cel. Agostinho, 76 - Sala 408 - Campo Grande, Rio de Janeiro - RJ, 23050-360</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>(21) 98493-0549</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>bityli.com</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Ajuste da mensagem do whatsapp E no tempo de envio pelo wpp web
</commit_message>
<xml_diff>
--- a/company_data.xlsx
+++ b/company_data.xlsx
@@ -463,22 +463,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Be Odonto</t>
+          <t>Bruno Cortes - Marketing Digital</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Office Mall Campo Grande - Estrada do Cachamorra, 350. Bloco 1, sala 423 - Campo Grande, Rio de Janeiro - RJ, 23040-150</t>
+          <t>Estr. da Cachamorra, 1233 - Campo Grande, Rio de Janeiro - RJ, 23040-150</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>(21) 96681-8555</t>
+          <t>(21) 98836-0205</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>beodontologia.com.br</t>
+          <t>brunocortes.com.br</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -486,60 +486,56 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Gal Odontologia</t>
+          <t>Winner Digital Pro | Agencia de Marketing Digital | Gestor de Trafego | Criação de Sites | Social Media</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Av. Belmiro Valverde, 87 - Campo Grande, Rio de Janeiro - RJ, 23010-540</t>
+          <t>R. Gramado, 475 - Campo Grande, Rio de Janeiro - RJ, 23050-090</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(21) 97469-6436</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+          <t>(21) 98552-3425</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>winnerdigitalpro.com</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>K.A. Clínica de Odontologia e Estética</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Estr. do Monteiro, 244 - Sala 207 - Campo Grande, Rio de Janeiro - RJ, 23045-830</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>(21) 97544-0520</t>
-        </is>
-      </c>
+          <t>RAES Marketing Digital</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Clínica Dra Priscila Máximo - Odontopediatria Campo Grande RJ / Invisalign</t>
+          <t>Bruno Cortes - Marketing Digital</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Av. Maria Teresa, 260 - Bl3 Sl 320 - Campo Grande, Rio de Janeiro - RJ, 23050-160</t>
+          <t>Estr. da Cachamorra, 1233 - Campo Grande, Rio de Janeiro - RJ, 23040-150</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>(21) 99883-0999</t>
+          <t>(21) 98836-0205</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>instagram.com</t>
+          <t>brunocortes.com.br</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -547,79 +543,87 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Odonto Nobre Rio</t>
+          <t>E-mind Negócios Digitais</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Estrada da Cachamorra. 350 bl:03 loja:127 - Campo Grande, Rio de Janeiro - RJ, 23040-150</t>
+          <t>Estr. da Cachamorra, 350 - Bloco 1 Sala 415 - Campo Grande, Rio de Janeiro - RJ, 23040-150</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>(21) 2412-5522</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
+          <t>(21) 96640-2049</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>emindnegocios.com.br</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Dra Graciele Castro - Odontologia</t>
+          <t>New Digital | Agencia de Marketing Digital | Gestor de Trafego | Criação de Sites</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Estr. da Cachamorra, 350 - bloco 3 sala 204 - Campo Grande, Rio de Janeiro - RJ, 23040-150</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+          <t>Centro Comercial Business Completo, Av. Maria Teresa, 75 - Campo Grande, Rio de Janeiro - RJ, 23050-160</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>(21) 99880-4831</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>newdigitalpro.com.br</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sorrisos Odontologia</t>
+          <t>Agência e Produtora Páginas e Aplicativos</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R. Prof. Castilho, 431 - Loja N - Campo Grande, Rio de Janeiro - RJ, 23045-060</t>
+          <t>Office Mall - RJ - Estr. da Cachamorra, 350 - Bloco 3 - Sala 461 - Campo Grande, Rio de Janeiro - RJ, 23040-150</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>(21) 3281-4872</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>sorrisosodontologia.com.br</t>
-        </is>
-      </c>
+          <t>(21) 98046-3733</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Sorrisart - Clínica e Emergência Odontológica</t>
+          <t>Agência de Marketing Digital - BeHype Media</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R. Augusto de Vasconcelos, 177 - Salas 408 a 410 - Campo Grande, Rio de Janeiro - RJ, 23050-340</t>
+          <t>Av. Maria Teresa, 260 - Campo Grande, Rio de Janeiro - RJ, 23050-160</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>(21) 97906-4001</t>
+          <t>(21) 97585-6922</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>sorrisart.com</t>
+          <t>behypemedia.com</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -627,45 +631,37 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Odontoclínica Campo Grande</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Rua Coronel Agostinho, 76 2º andar, sobrelojas 206, 213, 215 e 217 - Campo Grande, Rio de Janeiro - RJ, 23050-360</t>
-        </is>
-      </c>
+          <t>Agência de Marketing Digital | Ouro Space</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>(21) 3402-1227</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>odontoclinicacg.com.br</t>
-        </is>
-      </c>
+          <t>(21) 97274-1361</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Multiodonto Clinica Odontológica</t>
+          <t>TM Group - Agência de Marketing</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R. Cel. Agostinho, 76 - Sala 408 - Campo Grande, Rio de Janeiro - RJ, 23050-360</t>
+          <t>R. Vicente Perrota - Campo Grande, Rio de Janeiro - RJ, 23036-180</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>(21) 98493-0549</t>
+          <t>(21) 97949-3723</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>bityli.com</t>
+          <t>agenciatmgroup.com.br</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>

</xml_diff>